<commit_message>
changes to registration page
</commit_message>
<xml_diff>
--- a/data/Masterdata.xlsx
+++ b/data/Masterdata.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -14,12 +14,12 @@
     <sheet name="Shop_SummerDress" sheetId="5" r:id="rId5"/>
     <sheet name="Shop_Tshirt" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="193">
   <si>
     <t>First name</t>
   </si>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1596,7 +1596,9 @@
       <c r="O11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="P11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
@@ -1644,7 +1646,9 @@
       <c r="O12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P12" s="2"/>
+      <c r="P12" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
@@ -1692,7 +1696,9 @@
       <c r="O13" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="P13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
@@ -1740,7 +1746,9 @@
       <c r="O14" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="P14" s="2"/>
+      <c r="P14" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
@@ -1788,7 +1796,9 @@
       <c r="O15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="P15" s="2"/>
+      <c r="P15" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
@@ -1836,7 +1846,9 @@
       <c r="O16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="P16" s="2"/>
+      <c r="P16" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="2" t="s">
@@ -1884,7 +1896,9 @@
       <c r="O17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="P17" s="2"/>
+      <c r="P17" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="2" t="s">

</xml_diff>

<commit_message>
fix registration issue related to excel sheet updat
</commit_message>
<xml_diff>
--- a/data/Masterdata.xlsx
+++ b/data/Masterdata.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="2" r:id="rId1"/>
-    <sheet name="registration" sheetId="1" r:id="rId2"/>
-    <sheet name="Shop_Blouse" sheetId="3" r:id="rId3"/>
-    <sheet name="Shop_EveningDress" sheetId="4" r:id="rId4"/>
-    <sheet name="Shop_SummerDress" sheetId="5" r:id="rId5"/>
-    <sheet name="Shop_Tshirt" sheetId="6" r:id="rId6"/>
+    <sheet name="login" r:id="rId1" sheetId="2"/>
+    <sheet name="registration" r:id="rId2" sheetId="1"/>
+    <sheet name="Shop_Blouse" r:id="rId3" sheetId="3"/>
+    <sheet name="Shop_EveningDress" r:id="rId4" sheetId="4"/>
+    <sheet name="Shop_SummerDress" r:id="rId5" sheetId="5"/>
+    <sheet name="Shop_Tshirt" r:id="rId6" sheetId="6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="273">
   <si>
     <t>First name</t>
   </si>
@@ -598,12 +598,253 @@
   </si>
   <si>
     <t>Short Sleeve</t>
+  </si>
+  <si>
+    <t>Khanb</t>
+  </si>
+  <si>
+    <t>Khanc</t>
+  </si>
+  <si>
+    <t>Khand</t>
+  </si>
+  <si>
+    <t>Khane</t>
+  </si>
+  <si>
+    <t>Khanf</t>
+  </si>
+  <si>
+    <t>Khang</t>
+  </si>
+  <si>
+    <t>Khanh</t>
+  </si>
+  <si>
+    <t>Khani</t>
+  </si>
+  <si>
+    <t>Khanj</t>
+  </si>
+  <si>
+    <t>fname19@gmail.com</t>
+  </si>
+  <si>
+    <t>fname20@gmail.com</t>
+  </si>
+  <si>
+    <t>fname21@gmail.com</t>
+  </si>
+  <si>
+    <t>fname22@gmail.com</t>
+  </si>
+  <si>
+    <t>fname23@gmail.com</t>
+  </si>
+  <si>
+    <t>fname24@gmail.com</t>
+  </si>
+  <si>
+    <t>fname25@gmail.com</t>
+  </si>
+  <si>
+    <t>fname26@gmail.com</t>
+  </si>
+  <si>
+    <t>fname27@gmail.com</t>
+  </si>
+  <si>
+    <t>23/5/1996</t>
+  </si>
+  <si>
+    <t>23/5/1997</t>
+  </si>
+  <si>
+    <t>23/5/1998</t>
+  </si>
+  <si>
+    <t>23/5/1999</t>
+  </si>
+  <si>
+    <t>23/5/2000</t>
+  </si>
+  <si>
+    <t>23/5/2001</t>
+  </si>
+  <si>
+    <t>23/5/2002</t>
+  </si>
+  <si>
+    <t>23/5/2003</t>
+  </si>
+  <si>
+    <t>test@1234585</t>
+  </si>
+  <si>
+    <t>test@1234586</t>
+  </si>
+  <si>
+    <t>test@1234587</t>
+  </si>
+  <si>
+    <t>test@1234588</t>
+  </si>
+  <si>
+    <t>test@1234589</t>
+  </si>
+  <si>
+    <t>test@1234590</t>
+  </si>
+  <si>
+    <t>test@1234591</t>
+  </si>
+  <si>
+    <t>test@1234592</t>
+  </si>
+  <si>
+    <t>test@1234593</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet19</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet20</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet21</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet22</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet23</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet24</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet25</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet26</t>
+  </si>
+  <si>
+    <t>address1,po1,lstreet27</t>
+  </si>
+  <si>
+    <t>Address30</t>
+  </si>
+  <si>
+    <t>Address31</t>
+  </si>
+  <si>
+    <t>Address32</t>
+  </si>
+  <si>
+    <t>Address33</t>
+  </si>
+  <si>
+    <t>Address34</t>
+  </si>
+  <si>
+    <t>Address35</t>
+  </si>
+  <si>
+    <t>Address36</t>
+  </si>
+  <si>
+    <t>Address37</t>
+  </si>
+  <si>
+    <t>Address38</t>
+  </si>
+  <si>
+    <t>add info19</t>
+  </si>
+  <si>
+    <t>add info20</t>
+  </si>
+  <si>
+    <t>add info21</t>
+  </si>
+  <si>
+    <t>add info22</t>
+  </si>
+  <si>
+    <t>add info23</t>
+  </si>
+  <si>
+    <t>add info24</t>
+  </si>
+  <si>
+    <t>add info25</t>
+  </si>
+  <si>
+    <t>add info26</t>
+  </si>
+  <si>
+    <t>add info27</t>
+  </si>
+  <si>
+    <t>addressalias19</t>
+  </si>
+  <si>
+    <t>addressalias20</t>
+  </si>
+  <si>
+    <t>addressalias21</t>
+  </si>
+  <si>
+    <t>addressalias22</t>
+  </si>
+  <si>
+    <t>addressalias23</t>
+  </si>
+  <si>
+    <t>addressalias24</t>
+  </si>
+  <si>
+    <t>addressalias25</t>
+  </si>
+  <si>
+    <t>addressalias26</t>
+  </si>
+  <si>
+    <t>addressalias27</t>
+  </si>
+  <si>
+    <t>Debb</t>
+  </si>
+  <si>
+    <t>Debc</t>
+  </si>
+  <si>
+    <t>Debd</t>
+  </si>
+  <si>
+    <t>Debe</t>
+  </si>
+  <si>
+    <t>Debf</t>
+  </si>
+  <si>
+    <t>Debg</t>
+  </si>
+  <si>
+    <t>Debh</t>
+  </si>
+  <si>
+    <t>Debi</t>
+  </si>
+  <si>
+    <t>Debj</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -667,24 +908,24 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -693,10 +934,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -852,7 +1093,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -861,13 +1102,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -877,7 +1118,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -886,7 +1127,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -895,7 +1136,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -905,12 +1146,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -941,7 +1182,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -960,7 +1201,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -981,8 +1222,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1017,37 +1258,45 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="A2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -1946,7 +2195,9 @@
       <c r="O18" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P18" s="2"/>
+      <c r="P18" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="2" t="s">
@@ -1994,38 +2245,489 @@
       <c r="O19" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="P19" s="2"/>
+      <c r="P19" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="2">
+        <v>12363</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="N20" s="2">
+        <v>123456807</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="2">
+        <v>12364</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="N21" s="2">
+        <v>123456808</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K22" s="2">
+        <v>12365</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="N22" s="2">
+        <v>123456809</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="2">
+        <v>12366</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="N23" s="2">
+        <v>123456810</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="P23" s="2"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="2">
+        <v>12367</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="N24" s="2">
+        <v>123456811</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="2">
+        <v>12368</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="N25" s="2">
+        <v>123456812</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="P25" s="2"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K26" s="2">
+        <v>12369</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N26" s="2">
+        <v>123456813</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K27" s="2">
+        <v>12370</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="N27" s="2">
+        <v>123456814</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K28" s="2">
+        <v>12371</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="N28" s="2">
+        <v>123456815</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="P28" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F10" r:id="rId2" display="test@1234567"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D3:D10" r:id="rId4" display="fname1@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="D4" r:id="rId6"/>
-    <hyperlink ref="D5" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
-    <hyperlink ref="D7" r:id="rId9"/>
-    <hyperlink ref="D8" r:id="rId10"/>
-    <hyperlink ref="D9" r:id="rId11"/>
-    <hyperlink ref="D10" r:id="rId12"/>
-    <hyperlink ref="F3" r:id="rId13"/>
-    <hyperlink ref="D11:D19" r:id="rId14" display="fname9@gmail.com"/>
-    <hyperlink ref="D11" r:id="rId15"/>
-    <hyperlink ref="D12" r:id="rId16"/>
-    <hyperlink ref="D13" r:id="rId17"/>
-    <hyperlink ref="D14" r:id="rId18"/>
-    <hyperlink ref="D15" r:id="rId19"/>
-    <hyperlink ref="D16" r:id="rId20"/>
-    <hyperlink ref="D17" r:id="rId21"/>
-    <hyperlink ref="D18" r:id="rId22"/>
-    <hyperlink ref="D19" r:id="rId23"/>
-    <hyperlink ref="F11:F19" r:id="rId24" display="test@1234567"/>
-    <hyperlink ref="F9" r:id="rId25"/>
+    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink display="test@1234567" r:id="rId2" ref="F3:F10"/>
+    <hyperlink r:id="rId3" ref="D2"/>
+    <hyperlink display="fname1@gmail.com" r:id="rId4" ref="D3:D10"/>
+    <hyperlink r:id="rId5" ref="D3"/>
+    <hyperlink r:id="rId6" ref="D4"/>
+    <hyperlink r:id="rId7" ref="D5"/>
+    <hyperlink r:id="rId8" ref="D6"/>
+    <hyperlink r:id="rId9" ref="D7"/>
+    <hyperlink r:id="rId10" ref="D8"/>
+    <hyperlink r:id="rId11" ref="D9"/>
+    <hyperlink r:id="rId12" ref="D10"/>
+    <hyperlink r:id="rId13" ref="F3"/>
+    <hyperlink display="fname9@gmail.com" r:id="rId14" ref="D11:D19"/>
+    <hyperlink r:id="rId15" ref="D11"/>
+    <hyperlink r:id="rId16" ref="D12"/>
+    <hyperlink r:id="rId17" ref="D13"/>
+    <hyperlink r:id="rId18" ref="D14"/>
+    <hyperlink r:id="rId19" ref="D15"/>
+    <hyperlink r:id="rId20" ref="D16"/>
+    <hyperlink r:id="rId21" ref="D17"/>
+    <hyperlink r:id="rId22" ref="D18"/>
+    <hyperlink r:id="rId23" ref="D19"/>
+    <hyperlink display="test@1234567" r:id="rId24" ref="F11:F19"/>
+    <hyperlink r:id="rId25" ref="F9"/>
+    <hyperlink r:id="rId26" ref="D20"/>
+    <hyperlink r:id="rId27" ref="D21"/>
+    <hyperlink r:id="rId28" ref="D22"/>
+    <hyperlink r:id="rId29" ref="D23"/>
+    <hyperlink r:id="rId30" ref="D24"/>
+    <hyperlink r:id="rId31" ref="D25"/>
+    <hyperlink r:id="rId32" ref="D26"/>
+    <hyperlink r:id="rId33" ref="D27"/>
+    <hyperlink r:id="rId34" ref="D28"/>
+    <hyperlink r:id="rId35" ref="F20"/>
+    <hyperlink display="test@1234585" r:id="rId36" ref="F21:F28"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId37" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -2039,9 +2741,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2391,15 +3093,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A15" type="list">
       <formula1>"S,L,M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B15" type="list">
       <formula1>"White,Black"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -2413,9 +3115,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2765,15 +3467,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B15" type="list">
       <formula1>"White,Black"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A15" type="list">
       <formula1>"S,L,M"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -2787,9 +3489,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3139,15 +3841,15 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A15" type="list">
       <formula1>"S,L,M"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B15" type="list">
       <formula1>"White,Black"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -3161,9 +3863,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3513,14 +4215,14 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B15" type="list">
       <formula1>"White,Black"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2:A15" type="list">
       <formula1>"S,L,M"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After pulling maven dependency changes from repo,Executed from OFC,
</commit_message>
<xml_diff>
--- a/data/Masterdata.xlsx
+++ b/data/Masterdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="273">
   <si>
     <t>First name</t>
   </si>
@@ -1266,6 +1266,14 @@
         <v>221</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
@@ -1294,7 +1302,7 @@
     <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
@@ -2445,7 +2453,9 @@
       <c r="O23" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="P23" s="2"/>
+      <c r="P23" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="2" t="s">
@@ -2741,9 +2751,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3115,9 +3125,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3489,9 +3499,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3863,9 +3873,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>